<commit_message>
Update to tabOTTR 0.2. Support list values.
</commit_message>
<xml_diff>
--- a/lutra-tab/src/test/resources/test1.xlsx
+++ b/lutra-tab/src/test/resources/test1.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet1_2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
   <si>
     <t xml:space="preserve">#OTTR</t>
   </si>
@@ -32,23 +33,7 @@
     <t xml:space="preserve">ex</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">http://example.org</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">#</t>
-    </r>
+    <t xml:space="preserve">http://example.org#</t>
   </si>
   <si>
     <t xml:space="preserve">end</t>
@@ -120,23 +105,25 @@
     <t xml:space="preserve">ex2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">http://easdfasdfxample</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.org#</t>
-    </r>
+    <t xml:space="preserve">http://easdfasdfxample.org#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://candidate.ottr.xyz/owl/axiom/DisjointClasses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iri+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:ClassA1|ex:ClassA2|ex:ClassA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:ClassB1|ex:ClassB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:ClassC1|ex:ClassC2|ex:ClassC3|ex:ClassC4</t>
   </si>
 </sst>
 </file>
@@ -151,6 +138,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -172,6 +160,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -249,15 +238,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="C11 D8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -389,7 +377,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://example.org"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://example.org#"/>
     <hyperlink ref="C4" r:id="rId2" display="http://candidate.ottr.xyz/owl/axiom/SuperObjectMaxCardinality"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -409,16 +397,15 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,13 +564,118 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://example.org"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://example.org#"/>
     <hyperlink ref="C7" r:id="rId2" display="http://candidate.ottr.xyz/owl/axiom/SubObjectMinCardinality"/>
-    <hyperlink ref="B23" r:id="rId3" display="http://easdfasdfxample"/>
+    <hyperlink ref="B23" r:id="rId3" display="http://easdfasdfxample.org#"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://example.org#"/>
+    <hyperlink ref="C4" r:id="rId2" display="http://candidate.ottr.xyz/owl/axiom/DisjointClasses"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
fix(tabOTTR): :boom: Rearranging row order for template instruction. BREAKING CHANGE
</commit_message>
<xml_diff>
--- a/lutra-tab/src/test/resources/test1.xlsx
+++ b/lutra-tab/src/test/resources/test1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,6 +45,12 @@
     <t xml:space="preserve">http://candidate.ottr.xyz/owl/axiom/SuperObjectMaxCardinality</t>
   </si>
   <si>
+    <t xml:space="preserve">iri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsd:int</t>
+  </si>
+  <si>
     <t xml:space="preserve">class</t>
   </si>
   <si>
@@ -57,12 +63,6 @@
     <t xml:space="preserve">range</t>
   </si>
   <si>
-    <t xml:space="preserve">iri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xsd:int</t>
-  </si>
-  <si>
     <t xml:space="preserve">ex:ClassA1</t>
   </si>
   <si>
@@ -111,10 +111,10 @@
     <t xml:space="preserve">http://candidate.ottr.xyz/owl/axiom/DisjointClasses</t>
   </si>
   <si>
+    <t xml:space="preserve">iri+</t>
+  </si>
+  <si>
     <t xml:space="preserve">classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iri+</t>
   </si>
   <si>
     <t xml:space="preserve">ex:ClassA1|ex:ClassA2|ex:ClassA3</t>
@@ -238,14 +238,12 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,45 +282,45 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>4</v>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,15 +395,13 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,48 +440,48 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>1</v>
+      <c r="C9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,13 +581,13 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,14 +626,15 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">

</xml_diff>

<commit_message>
fix(tabOTTR): :boom: Change list separator to $$. BREAKING CHANGE
</commit_message>
<xml_diff>
--- a/lutra-tab/src/test/resources/test1.xlsx
+++ b/lutra-tab/src/test/resources/test1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -117,13 +117,13 @@
     <t xml:space="preserve">classes</t>
   </si>
   <si>
-    <t xml:space="preserve">ex:ClassA1|ex:ClassA2|ex:ClassA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ex:ClassB1|ex:ClassB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ex:ClassC1|ex:ClassC2|ex:ClassC3|ex:ClassC4</t>
+    <t xml:space="preserve">ex:ClassA1 $$ ex:ClassA2 $$ ex:ClassA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:ClassB1 $$ ex:ClassB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:ClassC1 $$ ex:ClassC2 $$ ex:ClassC3 $$ ex:ClassC4</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,13 +397,15 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,14 +585,11 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
feat(tabOTTR): :sparkles: support explicitly typed literals in auto
</commit_message>
<xml_diff>
--- a/lutra-tab/src/test/resources/test1.xlsx
+++ b/lutra-tab/src/test/resources/test1.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet1_2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="45">
   <si>
     <t xml:space="preserve">#OTTR</t>
   </si>
@@ -124,14 +125,48 @@
   </si>
   <si>
     <t xml:space="preserve">ex:ClassC1 $$ ex:ClassC2 $$ ex:ClassC3 $$ ex:ClassC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://candidate.ottr.xyz/rdf/Triple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdf^^xsd:normalizedString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -205,7 +240,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,6 +250,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,9 +282,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,9 +442,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,11 +624,14 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -679,4 +721,157 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://example.org#"/>
+    <hyperlink ref="C4" r:id="rId2" display="http://candidate.ottr.xyz/rdf/Triple"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>